<commit_message>
Uso de mayúsculas en nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion06/ESCALETA_CN_08_06_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion06/ESCALETA_CN_08_06_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado08\guion06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11760"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="236">
   <si>
     <t>Asignatura</t>
   </si>
@@ -417,9 +422,6 @@
   </si>
   <si>
     <t>La herencia en la especie humana y los árboles genealógicos</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: las leyes de Mendel</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Las leyes de Mendel</t>
@@ -663,9 +665,6 @@
     <t>Interactivo que trata la relación entre meiosis y reproducción sexual</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el ciclo y la reproducción celular</t>
-  </si>
-  <si>
     <t>Interactivo que expone los conceptos de genotipo y fenotipo</t>
   </si>
   <si>
@@ -711,9 +710,6 @@
     <t>Evalúa tus conocimientos acerca del tema Los fundamentos de genética</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los genes</t>
-  </si>
-  <si>
     <t>La primera imagen de menú lleva a la explicación de qué es un gen (un fragmento de ADN que tiene las instrucciones para hacer una proteína); aquí también se explica que los genes determinan en parte cómo somos. La segunda imgen lleva a la explicación de donde se ubican los genes (locus y cromosomas), y otra imagen de menú habla de los alelos. Dentro de esta última hay varias pantallas en donde se explica qué son alelos, qué es dominancia, recesividad y codominancia, y como se representan los genes (letras mayúsculas y minúsculas segúan sean dominantes o recesivos, y letras con superíndices para codominantes). Al final de la exposición hay un recurso M1B para relacionar términos con su significado (gen, alelo, codominancia, etc).</t>
   </si>
   <si>
@@ -723,27 +719,18 @@
     <t>Actividad sobre cromosomas y aberraciones cromosómicas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los cromosomas</t>
-  </si>
-  <si>
     <t>El número cromosómico y las aberraciones en los cromosomas</t>
   </si>
   <si>
     <t>Recurso M101A-03</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la herencia y el ambiente</t>
-  </si>
-  <si>
     <t>Recurso M101AP-01</t>
   </si>
   <si>
     <t>Banco de actividades: Fundamentos de genética</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la genética</t>
-  </si>
-  <si>
     <t>El material genético</t>
   </si>
   <si>
@@ -784,6 +771,21 @@
   </si>
   <si>
     <t>Mapa conceptual</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La genética</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los genes</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los cromosomas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El ciclo y la reproducción celular</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La herencia y el ambiente</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1583,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1743,7 @@
       </c>
       <c r="N3" s="20"/>
       <c r="O3" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P3" s="48" t="s">
         <v>19</v>
@@ -1750,16 +1752,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="T3" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="U3" s="23" t="s">
         <v>202</v>
-      </c>
-      <c r="T3" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="U3" s="23" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1780,7 +1782,7 @@
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="42" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="H4" s="30">
         <v>2</v>
@@ -1789,7 +1791,7 @@
         <v>97</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>69</v>
@@ -1802,7 +1804,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P4" s="46" t="s">
         <v>19</v>
@@ -1811,16 +1813,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="T4" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T4" s="47" t="s">
-        <v>208</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1841,7 +1843,7 @@
       </c>
       <c r="F5" s="39"/>
       <c r="G5" s="42" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="H5" s="30">
         <v>3</v>
@@ -1850,7 +1852,7 @@
         <v>94</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="K5" s="45" t="s">
         <v>69</v>
@@ -1863,7 +1865,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="P5" s="46" t="s">
         <v>19</v>
@@ -1872,16 +1874,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="T5" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="T5" s="47" t="s">
-        <v>205</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1902,7 +1904,7 @@
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="42" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="H6" s="30">
         <v>4</v>
@@ -1931,16 +1933,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="T6" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T6" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1961,7 +1963,7 @@
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="42" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="H7" s="30">
         <v>5</v>
@@ -1970,7 +1972,7 @@
         <v>97</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K7" s="45" t="s">
         <v>69</v>
@@ -1983,7 +1985,7 @@
         <v>62</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="P7" s="46" t="s">
         <v>19</v>
@@ -1992,16 +1994,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S7" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="T7" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T7" s="47" t="s">
-        <v>209</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2042,7 +2044,7 @@
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P8" s="46" t="s">
         <v>19</v>
@@ -2088,7 +2090,7 @@
         <v>97</v>
       </c>
       <c r="J9" s="43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K9" s="45" t="s">
         <v>70</v>
@@ -2132,13 +2134,13 @@
         <v>102</v>
       </c>
       <c r="E10" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>192</v>
-      </c>
       <c r="G10" s="42" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H10" s="30">
         <v>8</v>
@@ -2147,7 +2149,7 @@
         <v>94</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K10" s="45" t="s">
         <v>69</v>
@@ -2160,7 +2162,7 @@
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P10" s="46" t="s">
         <v>19</v>
@@ -2169,16 +2171,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="S10" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="U10" s="36" t="s">
         <v>202</v>
-      </c>
-      <c r="T10" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="U10" s="36" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2195,13 +2197,13 @@
         <v>102</v>
       </c>
       <c r="E11" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="F11" s="39" t="s">
-        <v>192</v>
-      </c>
       <c r="G11" s="42" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H11" s="30">
         <v>9</v>
@@ -2210,7 +2212,7 @@
         <v>97</v>
       </c>
       <c r="J11" s="43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K11" s="45" t="s">
         <v>69</v>
@@ -2230,16 +2232,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S11" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S11" s="11" t="s">
+      <c r="T11" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T11" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2260,7 +2262,7 @@
       </c>
       <c r="F12" s="39"/>
       <c r="G12" s="42" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="H12" s="30">
         <v>10</v>
@@ -2269,7 +2271,7 @@
         <v>97</v>
       </c>
       <c r="J12" s="43" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K12" s="45" t="s">
         <v>69</v>
@@ -2289,16 +2291,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="S12" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="S12" s="27" t="s">
+      <c r="T12" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="U12" s="36" t="s">
         <v>156</v>
-      </c>
-      <c r="T12" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="U12" s="36" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2328,7 +2330,7 @@
         <v>94</v>
       </c>
       <c r="J13" s="43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K13" s="45" t="s">
         <v>70</v>
@@ -2385,7 +2387,7 @@
         <v>94</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" s="45" t="s">
         <v>70</v>
@@ -2499,7 +2501,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K16" s="45" t="s">
         <v>70</v>
@@ -2604,7 +2606,7 @@
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="42" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="H18" s="30">
         <v>16</v>
@@ -2613,7 +2615,7 @@
         <v>97</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K18" s="45" t="s">
         <v>70</v>
@@ -2657,11 +2659,11 @@
         <v>121</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="42" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H19" s="30">
         <v>17</v>
@@ -2670,7 +2672,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="43" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K19" s="45" t="s">
         <v>69</v>
@@ -2683,7 +2685,7 @@
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P19" s="46" t="s">
         <v>19</v>
@@ -2692,16 +2694,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="S19" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2718,11 +2720,11 @@
         <v>121</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="42" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H20" s="30">
         <v>18</v>
@@ -2731,7 +2733,7 @@
         <v>97</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K20" s="45" t="s">
         <v>70</v>
@@ -2779,7 +2781,7 @@
       </c>
       <c r="F21" s="39"/>
       <c r="G21" s="42" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="H21" s="30">
         <v>19</v>
@@ -2788,7 +2790,7 @@
         <v>97</v>
       </c>
       <c r="J21" s="43" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="K21" s="45" t="s">
         <v>69</v>
@@ -2808,16 +2810,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S21" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S21" s="11" t="s">
+      <c r="T21" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T21" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2849,7 +2851,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="K22" s="45" t="s">
         <v>70</v>
@@ -2956,7 +2958,7 @@
       </c>
       <c r="F24" s="39"/>
       <c r="G24" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" s="30">
         <v>22</v>
@@ -2965,7 +2967,7 @@
         <v>94</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K24" s="45" t="s">
         <v>70</v>
@@ -3013,7 +3015,7 @@
       </c>
       <c r="F25" s="39"/>
       <c r="G25" s="42" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H25" s="30">
         <v>23</v>
@@ -3022,7 +3024,7 @@
         <v>97</v>
       </c>
       <c r="J25" s="43" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="K25" s="45" t="s">
         <v>69</v>
@@ -3035,7 +3037,7 @@
         <v>23</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="P25" s="46" t="s">
         <v>20</v>
@@ -3044,16 +3046,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="S25" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="S25" s="28" t="s">
+      <c r="T25" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="U25" s="37" t="s">
         <v>156</v>
-      </c>
-      <c r="T25" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="U25" s="37" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3083,7 +3085,7 @@
         <v>97</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K26" s="45" t="s">
         <v>70</v>
@@ -3107,7 +3109,7 @@
         <v>93</v>
       </c>
       <c r="T26" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U26" s="37" t="s">
         <v>123</v>
@@ -3124,12 +3126,12 @@
         <v>92</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="39"/>
       <c r="G27" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H27" s="30">
         <v>25</v>
@@ -3138,7 +3140,7 @@
         <v>97</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K27" s="45" t="s">
         <v>70</v>
@@ -3162,7 +3164,7 @@
         <v>93</v>
       </c>
       <c r="T27" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U27" s="37" t="s">
         <v>123</v>
@@ -3179,12 +3181,12 @@
         <v>92</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="39"/>
       <c r="G28" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" s="30">
         <v>26</v>
@@ -3193,7 +3195,7 @@
         <v>97</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K28" s="45" t="s">
         <v>70</v>
@@ -3217,7 +3219,7 @@
         <v>93</v>
       </c>
       <c r="T28" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U28" s="37" t="s">
         <v>123</v>
@@ -3234,12 +3236,12 @@
         <v>92</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="39"/>
       <c r="G29" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H29" s="30">
         <v>27</v>
@@ -3248,7 +3250,7 @@
         <v>97</v>
       </c>
       <c r="J29" s="43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K29" s="45" t="s">
         <v>70</v>
@@ -3272,7 +3274,7 @@
         <v>93</v>
       </c>
       <c r="T29" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U29" s="37" t="s">
         <v>123</v>
@@ -3289,12 +3291,12 @@
         <v>92</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="29"/>
       <c r="F30" s="39"/>
       <c r="G30" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H30" s="30">
         <v>28</v>
@@ -3303,7 +3305,7 @@
         <v>97</v>
       </c>
       <c r="J30" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K30" s="45" t="s">
         <v>70</v>
@@ -3327,7 +3329,7 @@
         <v>106</v>
       </c>
       <c r="T30" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U30" s="37" t="s">
         <v>107</v>
@@ -3344,12 +3346,12 @@
         <v>92</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E31" s="29"/>
       <c r="F31" s="39"/>
       <c r="G31" s="42" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H31" s="30">
         <v>29</v>
@@ -3358,7 +3360,7 @@
         <v>97</v>
       </c>
       <c r="J31" s="43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K31" s="45" t="s">
         <v>69</v>
@@ -3389,12 +3391,12 @@
         <v>92</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="39"/>
       <c r="G32" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H32" s="30">
         <v>30</v>
@@ -3403,7 +3405,7 @@
         <v>97</v>
       </c>
       <c r="J32" s="43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K32" s="45" t="s">
         <v>69</v>
@@ -3423,16 +3425,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S32" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S32" s="11" t="s">
+      <c r="T32" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="U32" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T32" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3446,12 +3448,12 @@
         <v>92</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="39"/>
       <c r="G33" s="42" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H33" s="30">
         <v>31</v>
@@ -3460,7 +3462,7 @@
         <v>97</v>
       </c>
       <c r="J33" s="43" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K33" s="45" t="s">
         <v>69</v>
@@ -3480,25 +3482,20 @@
         <v>6</v>
       </c>
       <c r="R33" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="S33" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S33" s="11" t="s">
+      <c r="T33" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="U33" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T33" s="47" t="s">
-        <v>220</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3514,6 +3511,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4279,7 +4281,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H3" s="19"/>
     </row>
@@ -4301,7 +4303,7 @@
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -4323,7 +4325,7 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" s="8"/>
     </row>
@@ -4345,10 +4347,10 @@
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4369,10 +4371,10 @@
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4393,10 +4395,10 @@
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4417,10 +4419,10 @@
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4441,10 +4443,10 @@
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,10 +4467,10 @@
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4489,10 +4491,10 @@
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4515,10 +4517,10 @@
         <v>126</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4541,10 +4543,10 @@
         <v>126</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4567,10 +4569,10 @@
         <v>126</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4593,10 +4595,10 @@
         <v>126</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4617,10 +4619,10 @@
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>